<commit_message>
Hashes of the sobel
</commit_message>
<xml_diff>
--- a/Reports/test data 2 (version2).xlsx
+++ b/Reports/test data 2 (version2).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="9495" windowHeight="13035" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="9495" windowHeight="13035" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
     <sheet name="Лист5" sheetId="5" r:id="rId5"/>
-    <sheet name="Лист6" sheetId="6" r:id="rId6"/>
-    <sheet name="Лист7" sheetId="7" r:id="rId7"/>
+    <sheet name="Wavelet coef" sheetId="6" r:id="rId6"/>
+    <sheet name="Sobel" sheetId="7" r:id="rId7"/>
+    <sheet name="Sobel hashes" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName name="log_" localSheetId="6">Sobel!$E$4:$O$67</definedName>
+    <definedName name="log_" localSheetId="7">'Sobel hashes'!$E$6:$O$69</definedName>
     <definedName name="log_" localSheetId="3">Лист4!$E$7:$O$73</definedName>
     <definedName name="log_" localSheetId="4">Лист5!$E$5:$O$69</definedName>
-    <definedName name="log_" localSheetId="6">Лист7!$E$4:$O$67</definedName>
     <definedName name="log__1" localSheetId="2">Лист3!$D$63:$N$130</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
@@ -96,11 +98,28 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="5" name="log_4" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="866" sourceFile="C:\Git\sift\log_.txt" decimal="," thousands=" " tab="0" space="1" consecutive="1">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="39">
   <si>
     <t>c_vector</t>
   </si>
@@ -203,12 +222,27 @@
   <si>
     <t>0.158</t>
   </si>
+  <si>
+    <t>sobel input</t>
+  </si>
+  <si>
+    <t>0.313</t>
+  </si>
+  <si>
+    <t>0.336</t>
+  </si>
+  <si>
+    <t>0.323</t>
+  </si>
+  <si>
+    <t>0.308</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,8 +282,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +301,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -275,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -285,6 +333,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -309,6 +359,10 @@
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="log_" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="log_" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3400,8 +3454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B63:AL179"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="N117" sqref="N117"/>
+    <sheetView topLeftCell="J57" workbookViewId="0">
+      <selection activeCell="AC67" sqref="AC67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10928,10 +10982,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="E4:AF38"/>
+  <dimension ref="E2:AF38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE20" sqref="AE20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10956,6 +11010,11 @@
     <col min="30" max="30" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="5:32">
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="4" spans="5:32">
       <c r="E4" t="s">
         <v>4</v>
@@ -12493,4 +12552,3307 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="E6:AM54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="Y41" sqref="Y41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="5:39">
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" t="s">
+        <v>5</v>
+      </c>
+      <c r="S6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="5:39">
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
+        <v>7</v>
+      </c>
+      <c r="S7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="5:39">
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>7</v>
+      </c>
+      <c r="S8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="5:39">
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>905</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9" t="s">
+        <v>7</v>
+      </c>
+      <c r="S9">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="10" spans="5:39">
+      <c r="F10">
+        <v>1632620</v>
+      </c>
+      <c r="G10">
+        <v>2115719</v>
+      </c>
+      <c r="H10">
+        <v>1435879</v>
+      </c>
+      <c r="I10">
+        <v>1288968</v>
+      </c>
+      <c r="J10">
+        <v>1220242</v>
+      </c>
+      <c r="K10">
+        <v>1170270</v>
+      </c>
+      <c r="L10">
+        <v>1163989</v>
+      </c>
+      <c r="M10">
+        <v>1391183</v>
+      </c>
+      <c r="N10">
+        <v>2112376</v>
+      </c>
+      <c r="O10">
+        <v>967820</v>
+      </c>
+      <c r="R10">
+        <v>1456884</v>
+      </c>
+      <c r="S10">
+        <v>1853133</v>
+      </c>
+      <c r="T10">
+        <v>1316086</v>
+      </c>
+      <c r="U10">
+        <v>1197141</v>
+      </c>
+      <c r="V10">
+        <v>1169702</v>
+      </c>
+      <c r="W10">
+        <v>1172236</v>
+      </c>
+      <c r="X10">
+        <v>1205056</v>
+      </c>
+      <c r="Y10">
+        <v>1444932</v>
+      </c>
+      <c r="Z10">
+        <v>2172708</v>
+      </c>
+      <c r="AA10">
+        <v>983117</v>
+      </c>
+      <c r="AD10">
+        <f>ABS(F10-R10)</f>
+        <v>175736</v>
+      </c>
+      <c r="AE10">
+        <f>ABS(G10-S10)</f>
+        <v>262586</v>
+      </c>
+      <c r="AF10">
+        <f>ABS(H10-T10)</f>
+        <v>119793</v>
+      </c>
+      <c r="AG10">
+        <f>ABS(I10-U10)</f>
+        <v>91827</v>
+      </c>
+      <c r="AH10">
+        <f>ABS(J10-V10)</f>
+        <v>50540</v>
+      </c>
+      <c r="AI10">
+        <f>ABS(K10-W10)</f>
+        <v>1966</v>
+      </c>
+      <c r="AJ10">
+        <f>ABS(L10-X10)</f>
+        <v>41067</v>
+      </c>
+      <c r="AK10">
+        <f>ABS(M10-Y10)</f>
+        <v>53749</v>
+      </c>
+      <c r="AL10">
+        <f>ABS(N10-Z10)</f>
+        <v>60332</v>
+      </c>
+      <c r="AM10">
+        <f>ABS(O10-AA10)</f>
+        <v>15297</v>
+      </c>
+    </row>
+    <row r="11" spans="5:39">
+      <c r="F11">
+        <v>2903602</v>
+      </c>
+      <c r="G11">
+        <v>1899477</v>
+      </c>
+      <c r="H11">
+        <v>1046306</v>
+      </c>
+      <c r="I11">
+        <v>949155</v>
+      </c>
+      <c r="J11">
+        <v>951624</v>
+      </c>
+      <c r="K11">
+        <v>906920</v>
+      </c>
+      <c r="L11">
+        <v>912484</v>
+      </c>
+      <c r="M11">
+        <v>1364010</v>
+      </c>
+      <c r="N11">
+        <v>2597731</v>
+      </c>
+      <c r="O11">
+        <v>2293763</v>
+      </c>
+      <c r="R11">
+        <v>2450766</v>
+      </c>
+      <c r="S11">
+        <v>1825274</v>
+      </c>
+      <c r="T11">
+        <v>968856</v>
+      </c>
+      <c r="U11">
+        <v>789244</v>
+      </c>
+      <c r="V11">
+        <v>874272</v>
+      </c>
+      <c r="W11">
+        <v>920212</v>
+      </c>
+      <c r="X11">
+        <v>981696</v>
+      </c>
+      <c r="Y11">
+        <v>1458497</v>
+      </c>
+      <c r="Z11">
+        <v>2678905</v>
+      </c>
+      <c r="AA11">
+        <v>2359312</v>
+      </c>
+      <c r="AD11">
+        <f>ABS(F11-R11)</f>
+        <v>452836</v>
+      </c>
+      <c r="AE11">
+        <f>ABS(G11-S11)</f>
+        <v>74203</v>
+      </c>
+      <c r="AF11">
+        <f>ABS(H11-T11)</f>
+        <v>77450</v>
+      </c>
+      <c r="AG11">
+        <f>ABS(I11-U11)</f>
+        <v>159911</v>
+      </c>
+      <c r="AH11">
+        <f>ABS(J11-V11)</f>
+        <v>77352</v>
+      </c>
+      <c r="AI11">
+        <f>ABS(K11-W11)</f>
+        <v>13292</v>
+      </c>
+      <c r="AJ11">
+        <f>ABS(L11-X11)</f>
+        <v>69212</v>
+      </c>
+      <c r="AK11">
+        <f>ABS(M11-Y11)</f>
+        <v>94487</v>
+      </c>
+      <c r="AL11">
+        <f>ABS(N11-Z11)</f>
+        <v>81174</v>
+      </c>
+      <c r="AM11">
+        <f>ABS(O11-AA11)</f>
+        <v>65549</v>
+      </c>
+    </row>
+    <row r="12" spans="5:39">
+      <c r="F12">
+        <v>2161627</v>
+      </c>
+      <c r="G12">
+        <v>1023729</v>
+      </c>
+      <c r="H12">
+        <v>318892</v>
+      </c>
+      <c r="I12">
+        <v>237461</v>
+      </c>
+      <c r="J12">
+        <v>167253</v>
+      </c>
+      <c r="K12">
+        <v>90554</v>
+      </c>
+      <c r="L12">
+        <v>92189</v>
+      </c>
+      <c r="M12">
+        <v>347942</v>
+      </c>
+      <c r="N12">
+        <v>1805487</v>
+      </c>
+      <c r="O12">
+        <v>1698917</v>
+      </c>
+      <c r="R12">
+        <v>1788236</v>
+      </c>
+      <c r="S12">
+        <v>860400</v>
+      </c>
+      <c r="T12">
+        <v>119530</v>
+      </c>
+      <c r="U12">
+        <v>96555</v>
+      </c>
+      <c r="V12">
+        <v>137034</v>
+      </c>
+      <c r="W12">
+        <v>98768</v>
+      </c>
+      <c r="X12">
+        <v>115978</v>
+      </c>
+      <c r="Y12">
+        <v>409459</v>
+      </c>
+      <c r="Z12">
+        <v>1918307</v>
+      </c>
+      <c r="AA12">
+        <v>1733855</v>
+      </c>
+      <c r="AD12">
+        <f>ABS(F12-R12)</f>
+        <v>373391</v>
+      </c>
+      <c r="AE12">
+        <f>ABS(G12-S12)</f>
+        <v>163329</v>
+      </c>
+      <c r="AF12">
+        <f>ABS(H12-T12)</f>
+        <v>199362</v>
+      </c>
+      <c r="AG12">
+        <f>ABS(I12-U12)</f>
+        <v>140906</v>
+      </c>
+      <c r="AH12">
+        <f>ABS(J12-V12)</f>
+        <v>30219</v>
+      </c>
+      <c r="AI12">
+        <f>ABS(K12-W12)</f>
+        <v>8214</v>
+      </c>
+      <c r="AJ12">
+        <f>ABS(L12-X12)</f>
+        <v>23789</v>
+      </c>
+      <c r="AK12">
+        <f>ABS(M12-Y12)</f>
+        <v>61517</v>
+      </c>
+      <c r="AL12">
+        <f>ABS(N12-Z12)</f>
+        <v>112820</v>
+      </c>
+      <c r="AM12">
+        <f>ABS(O12-AA12)</f>
+        <v>34938</v>
+      </c>
+    </row>
+    <row r="13" spans="5:39">
+      <c r="F13">
+        <v>1989609</v>
+      </c>
+      <c r="G13">
+        <v>997484</v>
+      </c>
+      <c r="H13">
+        <v>277822</v>
+      </c>
+      <c r="I13">
+        <v>114872</v>
+      </c>
+      <c r="J13">
+        <v>38927</v>
+      </c>
+      <c r="K13">
+        <v>23499</v>
+      </c>
+      <c r="L13">
+        <v>39027</v>
+      </c>
+      <c r="M13">
+        <v>185496</v>
+      </c>
+      <c r="N13">
+        <v>1405030</v>
+      </c>
+      <c r="O13">
+        <v>1631648</v>
+      </c>
+      <c r="R13">
+        <v>1664488</v>
+      </c>
+      <c r="S13">
+        <v>615824</v>
+      </c>
+      <c r="T13">
+        <v>43414</v>
+      </c>
+      <c r="U13">
+        <v>19121</v>
+      </c>
+      <c r="V13">
+        <v>42510</v>
+      </c>
+      <c r="W13">
+        <v>31162</v>
+      </c>
+      <c r="X13">
+        <v>30084</v>
+      </c>
+      <c r="Y13">
+        <v>218605</v>
+      </c>
+      <c r="Z13">
+        <v>1672676</v>
+      </c>
+      <c r="AA13">
+        <v>1659503</v>
+      </c>
+      <c r="AD13">
+        <f>ABS(F13-R13)</f>
+        <v>325121</v>
+      </c>
+      <c r="AE13">
+        <f>ABS(G13-S13)</f>
+        <v>381660</v>
+      </c>
+      <c r="AF13">
+        <f>ABS(H13-T13)</f>
+        <v>234408</v>
+      </c>
+      <c r="AG13">
+        <f>ABS(I13-U13)</f>
+        <v>95751</v>
+      </c>
+      <c r="AH13">
+        <f>ABS(J13-V13)</f>
+        <v>3583</v>
+      </c>
+      <c r="AI13">
+        <f>ABS(K13-W13)</f>
+        <v>7663</v>
+      </c>
+      <c r="AJ13">
+        <f>ABS(L13-X13)</f>
+        <v>8943</v>
+      </c>
+      <c r="AK13">
+        <f>ABS(M13-Y13)</f>
+        <v>33109</v>
+      </c>
+      <c r="AL13">
+        <f>ABS(N13-Z13)</f>
+        <v>267646</v>
+      </c>
+      <c r="AM13">
+        <f>ABS(O13-AA13)</f>
+        <v>27855</v>
+      </c>
+    </row>
+    <row r="14" spans="5:39">
+      <c r="F14">
+        <v>1814981</v>
+      </c>
+      <c r="G14">
+        <v>1088220</v>
+      </c>
+      <c r="H14">
+        <v>269018</v>
+      </c>
+      <c r="I14">
+        <v>73478</v>
+      </c>
+      <c r="J14" s="10">
+        <v>34141</v>
+      </c>
+      <c r="K14" s="10">
+        <v>33455</v>
+      </c>
+      <c r="L14">
+        <v>35454</v>
+      </c>
+      <c r="M14">
+        <v>156861</v>
+      </c>
+      <c r="N14">
+        <v>1315849</v>
+      </c>
+      <c r="O14">
+        <v>1705262</v>
+      </c>
+      <c r="R14">
+        <v>1634866</v>
+      </c>
+      <c r="S14">
+        <v>680088</v>
+      </c>
+      <c r="T14">
+        <v>61321</v>
+      </c>
+      <c r="U14">
+        <v>22504</v>
+      </c>
+      <c r="V14" s="9">
+        <v>39198</v>
+      </c>
+      <c r="W14" s="9">
+        <v>40756</v>
+      </c>
+      <c r="X14">
+        <v>62541</v>
+      </c>
+      <c r="Y14">
+        <v>352524</v>
+      </c>
+      <c r="Z14">
+        <v>1669989</v>
+      </c>
+      <c r="AA14">
+        <v>1774384</v>
+      </c>
+      <c r="AD14">
+        <f>ABS(F14-R14)</f>
+        <v>180115</v>
+      </c>
+      <c r="AE14">
+        <f>ABS(G14-S14)</f>
+        <v>408132</v>
+      </c>
+      <c r="AF14">
+        <f>ABS(H14-T14)</f>
+        <v>207697</v>
+      </c>
+      <c r="AG14">
+        <f>ABS(I14-U14)</f>
+        <v>50974</v>
+      </c>
+      <c r="AH14">
+        <f>ABS(J14-V14)</f>
+        <v>5057</v>
+      </c>
+      <c r="AI14">
+        <f>ABS(K14-W14)</f>
+        <v>7301</v>
+      </c>
+      <c r="AJ14">
+        <f>ABS(L14-X14)</f>
+        <v>27087</v>
+      </c>
+      <c r="AK14">
+        <f>ABS(M14-Y14)</f>
+        <v>195663</v>
+      </c>
+      <c r="AL14">
+        <f>ABS(N14-Z14)</f>
+        <v>354140</v>
+      </c>
+      <c r="AM14">
+        <f>ABS(O14-AA14)</f>
+        <v>69122</v>
+      </c>
+    </row>
+    <row r="15" spans="5:39">
+      <c r="F15">
+        <v>1621893</v>
+      </c>
+      <c r="G15">
+        <v>1028034</v>
+      </c>
+      <c r="H15">
+        <v>149353</v>
+      </c>
+      <c r="I15">
+        <v>31903</v>
+      </c>
+      <c r="J15" s="10">
+        <v>44896</v>
+      </c>
+      <c r="K15" s="10">
+        <v>32929</v>
+      </c>
+      <c r="L15">
+        <v>21963</v>
+      </c>
+      <c r="M15">
+        <v>110749</v>
+      </c>
+      <c r="N15">
+        <v>1228405</v>
+      </c>
+      <c r="O15">
+        <v>1760224</v>
+      </c>
+      <c r="R15">
+        <v>1558795</v>
+      </c>
+      <c r="S15">
+        <v>767213</v>
+      </c>
+      <c r="T15">
+        <v>99913</v>
+      </c>
+      <c r="U15">
+        <v>31579</v>
+      </c>
+      <c r="V15" s="9">
+        <v>28704</v>
+      </c>
+      <c r="W15" s="9">
+        <v>42405</v>
+      </c>
+      <c r="X15">
+        <v>136090</v>
+      </c>
+      <c r="Y15">
+        <v>420420</v>
+      </c>
+      <c r="Z15">
+        <v>1562729</v>
+      </c>
+      <c r="AA15">
+        <v>1944206</v>
+      </c>
+      <c r="AD15">
+        <f>ABS(F15-R15)</f>
+        <v>63098</v>
+      </c>
+      <c r="AE15">
+        <f>ABS(G15-S15)</f>
+        <v>260821</v>
+      </c>
+      <c r="AF15">
+        <f>ABS(H15-T15)</f>
+        <v>49440</v>
+      </c>
+      <c r="AG15">
+        <f>ABS(I15-U15)</f>
+        <v>324</v>
+      </c>
+      <c r="AH15">
+        <f>ABS(J15-V15)</f>
+        <v>16192</v>
+      </c>
+      <c r="AI15">
+        <f>ABS(K15-W15)</f>
+        <v>9476</v>
+      </c>
+      <c r="AJ15">
+        <f>ABS(L15-X15)</f>
+        <v>114127</v>
+      </c>
+      <c r="AK15">
+        <f>ABS(M15-Y15)</f>
+        <v>309671</v>
+      </c>
+      <c r="AL15">
+        <f>ABS(N15-Z15)</f>
+        <v>334324</v>
+      </c>
+      <c r="AM15">
+        <f>ABS(O15-AA15)</f>
+        <v>183982</v>
+      </c>
+    </row>
+    <row r="16" spans="5:39">
+      <c r="F16">
+        <v>1521020</v>
+      </c>
+      <c r="G16">
+        <v>995232</v>
+      </c>
+      <c r="H16">
+        <v>83856</v>
+      </c>
+      <c r="I16">
+        <v>33927</v>
+      </c>
+      <c r="J16">
+        <v>45052</v>
+      </c>
+      <c r="K16">
+        <v>42760</v>
+      </c>
+      <c r="L16">
+        <v>23944</v>
+      </c>
+      <c r="M16">
+        <v>95829</v>
+      </c>
+      <c r="N16">
+        <v>1204975</v>
+      </c>
+      <c r="O16">
+        <v>1779449</v>
+      </c>
+      <c r="R16">
+        <v>1489652</v>
+      </c>
+      <c r="S16">
+        <v>833136</v>
+      </c>
+      <c r="T16">
+        <v>124135</v>
+      </c>
+      <c r="U16">
+        <v>36503</v>
+      </c>
+      <c r="V16">
+        <v>28978</v>
+      </c>
+      <c r="W16">
+        <v>76216</v>
+      </c>
+      <c r="X16">
+        <v>160763</v>
+      </c>
+      <c r="Y16">
+        <v>353082</v>
+      </c>
+      <c r="Z16">
+        <v>1377983</v>
+      </c>
+      <c r="AA16">
+        <v>2091385</v>
+      </c>
+      <c r="AD16">
+        <f>ABS(F16-R16)</f>
+        <v>31368</v>
+      </c>
+      <c r="AE16">
+        <f>ABS(G16-S16)</f>
+        <v>162096</v>
+      </c>
+      <c r="AF16">
+        <f>ABS(H16-T16)</f>
+        <v>40279</v>
+      </c>
+      <c r="AG16">
+        <f>ABS(I16-U16)</f>
+        <v>2576</v>
+      </c>
+      <c r="AH16">
+        <f>ABS(J16-V16)</f>
+        <v>16074</v>
+      </c>
+      <c r="AI16">
+        <f>ABS(K16-W16)</f>
+        <v>33456</v>
+      </c>
+      <c r="AJ16">
+        <f>ABS(L16-X16)</f>
+        <v>136819</v>
+      </c>
+      <c r="AK16">
+        <f>ABS(M16-Y16)</f>
+        <v>257253</v>
+      </c>
+      <c r="AL16">
+        <f>ABS(N16-Z16)</f>
+        <v>173008</v>
+      </c>
+      <c r="AM16">
+        <f>ABS(O16-AA16)</f>
+        <v>311936</v>
+      </c>
+    </row>
+    <row r="17" spans="5:39">
+      <c r="F17">
+        <v>1725550</v>
+      </c>
+      <c r="G17">
+        <v>1365783</v>
+      </c>
+      <c r="H17">
+        <v>391358</v>
+      </c>
+      <c r="I17">
+        <v>180749</v>
+      </c>
+      <c r="J17">
+        <v>180334</v>
+      </c>
+      <c r="K17">
+        <v>179954</v>
+      </c>
+      <c r="L17">
+        <v>126678</v>
+      </c>
+      <c r="M17">
+        <v>280144</v>
+      </c>
+      <c r="N17">
+        <v>1507136</v>
+      </c>
+      <c r="O17">
+        <v>1932745</v>
+      </c>
+      <c r="R17">
+        <v>1686762</v>
+      </c>
+      <c r="S17">
+        <v>1302152</v>
+      </c>
+      <c r="T17">
+        <v>306518</v>
+      </c>
+      <c r="U17">
+        <v>154738</v>
+      </c>
+      <c r="V17">
+        <v>198950</v>
+      </c>
+      <c r="W17">
+        <v>263952</v>
+      </c>
+      <c r="X17">
+        <v>303956</v>
+      </c>
+      <c r="Y17">
+        <v>422702</v>
+      </c>
+      <c r="Z17">
+        <v>1421883</v>
+      </c>
+      <c r="AA17">
+        <v>2258547</v>
+      </c>
+      <c r="AD17">
+        <f>ABS(F17-R17)</f>
+        <v>38788</v>
+      </c>
+      <c r="AE17">
+        <f>ABS(G17-S17)</f>
+        <v>63631</v>
+      </c>
+      <c r="AF17">
+        <f>ABS(H17-T17)</f>
+        <v>84840</v>
+      </c>
+      <c r="AG17">
+        <f>ABS(I17-U17)</f>
+        <v>26011</v>
+      </c>
+      <c r="AH17">
+        <f>ABS(J17-V17)</f>
+        <v>18616</v>
+      </c>
+      <c r="AI17">
+        <f>ABS(K17-W17)</f>
+        <v>83998</v>
+      </c>
+      <c r="AJ17">
+        <f>ABS(L17-X17)</f>
+        <v>177278</v>
+      </c>
+      <c r="AK17">
+        <f>ABS(M17-Y17)</f>
+        <v>142558</v>
+      </c>
+      <c r="AL17">
+        <f>ABS(N17-Z17)</f>
+        <v>85253</v>
+      </c>
+      <c r="AM17">
+        <f>ABS(O17-AA17)</f>
+        <v>325802</v>
+      </c>
+    </row>
+    <row r="18" spans="5:39">
+      <c r="F18">
+        <v>2542992</v>
+      </c>
+      <c r="G18">
+        <v>2501977</v>
+      </c>
+      <c r="H18">
+        <v>1737695</v>
+      </c>
+      <c r="I18">
+        <v>1398615</v>
+      </c>
+      <c r="J18">
+        <v>1326063</v>
+      </c>
+      <c r="K18">
+        <v>1207250</v>
+      </c>
+      <c r="L18">
+        <v>1128327</v>
+      </c>
+      <c r="M18">
+        <v>1403153</v>
+      </c>
+      <c r="N18">
+        <v>2531527</v>
+      </c>
+      <c r="O18">
+        <v>2688790</v>
+      </c>
+      <c r="R18">
+        <v>2484614</v>
+      </c>
+      <c r="S18">
+        <v>2417306</v>
+      </c>
+      <c r="T18">
+        <v>1635769</v>
+      </c>
+      <c r="U18">
+        <v>1333363</v>
+      </c>
+      <c r="V18">
+        <v>1340323</v>
+      </c>
+      <c r="W18">
+        <v>1303579</v>
+      </c>
+      <c r="X18">
+        <v>1235378</v>
+      </c>
+      <c r="Y18">
+        <v>1327681</v>
+      </c>
+      <c r="Z18">
+        <v>2385539</v>
+      </c>
+      <c r="AA18">
+        <v>3075934</v>
+      </c>
+      <c r="AD18">
+        <f>ABS(F18-R18)</f>
+        <v>58378</v>
+      </c>
+      <c r="AE18">
+        <f>ABS(G18-S18)</f>
+        <v>84671</v>
+      </c>
+      <c r="AF18">
+        <f>ABS(H18-T18)</f>
+        <v>101926</v>
+      </c>
+      <c r="AG18">
+        <f>ABS(I18-U18)</f>
+        <v>65252</v>
+      </c>
+      <c r="AH18">
+        <f>ABS(J18-V18)</f>
+        <v>14260</v>
+      </c>
+      <c r="AI18">
+        <f>ABS(K18-W18)</f>
+        <v>96329</v>
+      </c>
+      <c r="AJ18">
+        <f>ABS(L18-X18)</f>
+        <v>107051</v>
+      </c>
+      <c r="AK18">
+        <f>ABS(M18-Y18)</f>
+        <v>75472</v>
+      </c>
+      <c r="AL18">
+        <f>ABS(N18-Z18)</f>
+        <v>145988</v>
+      </c>
+      <c r="AM18">
+        <f>ABS(O18-AA18)</f>
+        <v>387144</v>
+      </c>
+    </row>
+    <row r="19" spans="5:39">
+      <c r="F19">
+        <v>1592428</v>
+      </c>
+      <c r="G19">
+        <v>2041210</v>
+      </c>
+      <c r="H19">
+        <v>1573686</v>
+      </c>
+      <c r="I19">
+        <v>1510835</v>
+      </c>
+      <c r="J19">
+        <v>1502986</v>
+      </c>
+      <c r="K19">
+        <v>1506846</v>
+      </c>
+      <c r="L19">
+        <v>1535144</v>
+      </c>
+      <c r="M19">
+        <v>1706170</v>
+      </c>
+      <c r="N19">
+        <v>2455137</v>
+      </c>
+      <c r="O19">
+        <v>1044390</v>
+      </c>
+      <c r="R19">
+        <v>1571871</v>
+      </c>
+      <c r="S19">
+        <v>1996878</v>
+      </c>
+      <c r="T19">
+        <v>1543110</v>
+      </c>
+      <c r="U19">
+        <v>1503582</v>
+      </c>
+      <c r="V19">
+        <v>1537680</v>
+      </c>
+      <c r="W19">
+        <v>1584077</v>
+      </c>
+      <c r="X19">
+        <v>1645370</v>
+      </c>
+      <c r="Y19">
+        <v>1810594</v>
+      </c>
+      <c r="Z19">
+        <v>2637175</v>
+      </c>
+      <c r="AA19">
+        <v>1066184</v>
+      </c>
+      <c r="AD19">
+        <f>ABS(F19-R19)</f>
+        <v>20557</v>
+      </c>
+      <c r="AE19">
+        <f>ABS(G19-S19)</f>
+        <v>44332</v>
+      </c>
+      <c r="AF19">
+        <f>ABS(H19-T19)</f>
+        <v>30576</v>
+      </c>
+      <c r="AG19">
+        <f>ABS(I19-U19)</f>
+        <v>7253</v>
+      </c>
+      <c r="AH19">
+        <f>ABS(J19-V19)</f>
+        <v>34694</v>
+      </c>
+      <c r="AI19">
+        <f>ABS(K19-W19)</f>
+        <v>77231</v>
+      </c>
+      <c r="AJ19">
+        <f>ABS(L19-X19)</f>
+        <v>110226</v>
+      </c>
+      <c r="AK19">
+        <f>ABS(M19-Y19)</f>
+        <v>104424</v>
+      </c>
+      <c r="AL19">
+        <f>ABS(N19-Z19)</f>
+        <v>182038</v>
+      </c>
+      <c r="AM19">
+        <f>ABS(O19-AA19)</f>
+        <v>21794</v>
+      </c>
+    </row>
+    <row r="20" spans="5:39">
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>100</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>3</v>
+      </c>
+      <c r="R20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="5:39">
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="5:39">
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" t="s">
+        <v>36</v>
+      </c>
+      <c r="J24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="5:39">
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>4</v>
+      </c>
+      <c r="R25" t="s">
+        <v>5</v>
+      </c>
+      <c r="S25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="5:39">
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26">
+        <v>10</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>1</v>
+      </c>
+      <c r="R26" t="s">
+        <v>7</v>
+      </c>
+      <c r="S26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="5:39">
+      <c r="E27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27">
+        <v>10</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>1</v>
+      </c>
+      <c r="R27" t="s">
+        <v>7</v>
+      </c>
+      <c r="S27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="5:39">
+      <c r="E28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <v>816</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>2</v>
+      </c>
+      <c r="R28" t="s">
+        <v>7</v>
+      </c>
+      <c r="S28">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="29" spans="5:39">
+      <c r="F29">
+        <v>1382304</v>
+      </c>
+      <c r="G29">
+        <v>1692456</v>
+      </c>
+      <c r="H29">
+        <v>1240470</v>
+      </c>
+      <c r="I29">
+        <v>1183654</v>
+      </c>
+      <c r="J29">
+        <v>1237160</v>
+      </c>
+      <c r="K29">
+        <v>1270334</v>
+      </c>
+      <c r="L29">
+        <v>1282136</v>
+      </c>
+      <c r="M29">
+        <v>1478672</v>
+      </c>
+      <c r="N29">
+        <v>2212596</v>
+      </c>
+      <c r="O29">
+        <v>960684</v>
+      </c>
+      <c r="R29">
+        <v>1411512</v>
+      </c>
+      <c r="S29">
+        <v>1738792</v>
+      </c>
+      <c r="T29">
+        <v>1272582</v>
+      </c>
+      <c r="U29">
+        <v>1230309</v>
+      </c>
+      <c r="V29">
+        <v>1350802</v>
+      </c>
+      <c r="W29">
+        <v>1490550</v>
+      </c>
+      <c r="X29">
+        <v>1575492</v>
+      </c>
+      <c r="Y29">
+        <v>1730112</v>
+      </c>
+      <c r="Z29">
+        <v>2495985</v>
+      </c>
+      <c r="AA29">
+        <v>1002590</v>
+      </c>
+      <c r="AD29">
+        <f>ABS(F29-R29)</f>
+        <v>29208</v>
+      </c>
+      <c r="AE29">
+        <f>ABS(G29-S29)</f>
+        <v>46336</v>
+      </c>
+      <c r="AF29">
+        <f>ABS(H29-T29)</f>
+        <v>32112</v>
+      </c>
+      <c r="AG29">
+        <f>ABS(I29-U29)</f>
+        <v>46655</v>
+      </c>
+      <c r="AH29">
+        <f>ABS(J29-V29)</f>
+        <v>113642</v>
+      </c>
+      <c r="AI29">
+        <f>ABS(K29-W29)</f>
+        <v>220216</v>
+      </c>
+      <c r="AJ29">
+        <f>ABS(L29-X29)</f>
+        <v>293356</v>
+      </c>
+      <c r="AK29">
+        <f>ABS(M29-Y29)</f>
+        <v>251440</v>
+      </c>
+      <c r="AL29">
+        <f>ABS(N29-Z29)</f>
+        <v>283389</v>
+      </c>
+      <c r="AM29">
+        <f>ABS(O29-AA29)</f>
+        <v>41906</v>
+      </c>
+    </row>
+    <row r="30" spans="5:39">
+      <c r="F30">
+        <v>2228821</v>
+      </c>
+      <c r="G30">
+        <v>2039509</v>
+      </c>
+      <c r="H30">
+        <v>1201374</v>
+      </c>
+      <c r="I30">
+        <v>846840</v>
+      </c>
+      <c r="J30">
+        <v>816663</v>
+      </c>
+      <c r="K30">
+        <v>739510</v>
+      </c>
+      <c r="L30">
+        <v>718966</v>
+      </c>
+      <c r="M30">
+        <v>1056335</v>
+      </c>
+      <c r="N30">
+        <v>2292179</v>
+      </c>
+      <c r="O30">
+        <v>2506836</v>
+      </c>
+      <c r="R30">
+        <v>2297084</v>
+      </c>
+      <c r="S30">
+        <v>2137201</v>
+      </c>
+      <c r="T30">
+        <v>1288023</v>
+      </c>
+      <c r="U30">
+        <v>1031559</v>
+      </c>
+      <c r="V30">
+        <v>1135575</v>
+      </c>
+      <c r="W30">
+        <v>1184196</v>
+      </c>
+      <c r="X30">
+        <v>1079830</v>
+      </c>
+      <c r="Y30">
+        <v>1193209</v>
+      </c>
+      <c r="Z30">
+        <v>2274806</v>
+      </c>
+      <c r="AA30">
+        <v>2851915</v>
+      </c>
+      <c r="AD30">
+        <f>ABS(F30-R30)</f>
+        <v>68263</v>
+      </c>
+      <c r="AE30">
+        <f>ABS(G30-S30)</f>
+        <v>97692</v>
+      </c>
+      <c r="AF30">
+        <f>ABS(H30-T30)</f>
+        <v>86649</v>
+      </c>
+      <c r="AG30">
+        <f>ABS(I30-U30)</f>
+        <v>184719</v>
+      </c>
+      <c r="AH30">
+        <f>ABS(J30-V30)</f>
+        <v>318912</v>
+      </c>
+      <c r="AI30">
+        <f>ABS(K30-W30)</f>
+        <v>444686</v>
+      </c>
+      <c r="AJ30">
+        <f>ABS(L30-X30)</f>
+        <v>360864</v>
+      </c>
+      <c r="AK30">
+        <f>ABS(M30-Y30)</f>
+        <v>136874</v>
+      </c>
+      <c r="AL30">
+        <f>ABS(N30-Z30)</f>
+        <v>17373</v>
+      </c>
+      <c r="AM30">
+        <f>ABS(O30-AA30)</f>
+        <v>345079</v>
+      </c>
+    </row>
+    <row r="31" spans="5:39">
+      <c r="F31">
+        <v>1592386</v>
+      </c>
+      <c r="G31">
+        <v>1122172</v>
+      </c>
+      <c r="H31">
+        <v>191673</v>
+      </c>
+      <c r="I31">
+        <v>125773</v>
+      </c>
+      <c r="J31">
+        <v>100693</v>
+      </c>
+      <c r="K31">
+        <v>59427</v>
+      </c>
+      <c r="L31">
+        <v>48053</v>
+      </c>
+      <c r="M31">
+        <v>204218</v>
+      </c>
+      <c r="N31">
+        <v>1410779</v>
+      </c>
+      <c r="O31">
+        <v>1829044</v>
+      </c>
+      <c r="R31">
+        <v>1650415</v>
+      </c>
+      <c r="S31">
+        <v>1222155</v>
+      </c>
+      <c r="T31">
+        <v>230962</v>
+      </c>
+      <c r="U31">
+        <v>84212</v>
+      </c>
+      <c r="V31">
+        <v>218483</v>
+      </c>
+      <c r="W31">
+        <v>319355</v>
+      </c>
+      <c r="X31">
+        <v>282163</v>
+      </c>
+      <c r="Y31">
+        <v>375672</v>
+      </c>
+      <c r="Z31">
+        <v>1364246</v>
+      </c>
+      <c r="AA31">
+        <v>2024583</v>
+      </c>
+      <c r="AD31">
+        <f>ABS(F31-R31)</f>
+        <v>58029</v>
+      </c>
+      <c r="AE31">
+        <f>ABS(G31-S31)</f>
+        <v>99983</v>
+      </c>
+      <c r="AF31">
+        <f>ABS(H31-T31)</f>
+        <v>39289</v>
+      </c>
+      <c r="AG31">
+        <f>ABS(I31-U31)</f>
+        <v>41561</v>
+      </c>
+      <c r="AH31">
+        <f>ABS(J31-V31)</f>
+        <v>117790</v>
+      </c>
+      <c r="AI31">
+        <f>ABS(K31-W31)</f>
+        <v>259928</v>
+      </c>
+      <c r="AJ31">
+        <f>ABS(L31-X31)</f>
+        <v>234110</v>
+      </c>
+      <c r="AK31">
+        <f>ABS(M31-Y31)</f>
+        <v>171454</v>
+      </c>
+      <c r="AL31">
+        <f>ABS(N31-Z31)</f>
+        <v>46533</v>
+      </c>
+      <c r="AM31">
+        <f>ABS(O31-AA31)</f>
+        <v>195539</v>
+      </c>
+    </row>
+    <row r="32" spans="5:39">
+      <c r="F32">
+        <v>1462837</v>
+      </c>
+      <c r="G32">
+        <v>791754</v>
+      </c>
+      <c r="H32">
+        <v>67699</v>
+      </c>
+      <c r="I32">
+        <v>27611</v>
+      </c>
+      <c r="J32">
+        <v>30061</v>
+      </c>
+      <c r="K32">
+        <v>19463</v>
+      </c>
+      <c r="L32">
+        <v>24888</v>
+      </c>
+      <c r="M32">
+        <v>139764</v>
+      </c>
+      <c r="N32">
+        <v>1246831</v>
+      </c>
+      <c r="O32">
+        <v>1685061</v>
+      </c>
+      <c r="R32">
+        <v>1489381</v>
+      </c>
+      <c r="S32">
+        <v>847458</v>
+      </c>
+      <c r="T32">
+        <v>77618</v>
+      </c>
+      <c r="U32">
+        <v>23018</v>
+      </c>
+      <c r="V32">
+        <v>43213</v>
+      </c>
+      <c r="W32">
+        <v>98651</v>
+      </c>
+      <c r="X32">
+        <v>127441</v>
+      </c>
+      <c r="Y32">
+        <v>291638</v>
+      </c>
+      <c r="Z32">
+        <v>1339068</v>
+      </c>
+      <c r="AA32">
+        <v>1826453</v>
+      </c>
+      <c r="AD32">
+        <f>ABS(F32-R32)</f>
+        <v>26544</v>
+      </c>
+      <c r="AE32">
+        <f>ABS(G32-S32)</f>
+        <v>55704</v>
+      </c>
+      <c r="AF32">
+        <f>ABS(H32-T32)</f>
+        <v>9919</v>
+      </c>
+      <c r="AG32">
+        <f>ABS(I32-U32)</f>
+        <v>4593</v>
+      </c>
+      <c r="AH32">
+        <f>ABS(J32-V32)</f>
+        <v>13152</v>
+      </c>
+      <c r="AI32">
+        <f>ABS(K32-W32)</f>
+        <v>79188</v>
+      </c>
+      <c r="AJ32">
+        <f>ABS(L32-X32)</f>
+        <v>102553</v>
+      </c>
+      <c r="AK32">
+        <f>ABS(M32-Y32)</f>
+        <v>151874</v>
+      </c>
+      <c r="AL32">
+        <f>ABS(N32-Z32)</f>
+        <v>92237</v>
+      </c>
+      <c r="AM32">
+        <f>ABS(O32-AA32)</f>
+        <v>141392</v>
+      </c>
+    </row>
+    <row r="33" spans="5:39">
+      <c r="F33">
+        <v>1521375</v>
+      </c>
+      <c r="G33">
+        <v>826483</v>
+      </c>
+      <c r="H33">
+        <v>93415</v>
+      </c>
+      <c r="I33">
+        <v>21286</v>
+      </c>
+      <c r="J33" s="10">
+        <v>33961</v>
+      </c>
+      <c r="K33" s="10">
+        <v>38504</v>
+      </c>
+      <c r="L33">
+        <v>48042</v>
+      </c>
+      <c r="M33">
+        <v>186532</v>
+      </c>
+      <c r="N33">
+        <v>1380008</v>
+      </c>
+      <c r="O33">
+        <v>1634080</v>
+      </c>
+      <c r="R33">
+        <v>1484545</v>
+      </c>
+      <c r="S33">
+        <v>825273</v>
+      </c>
+      <c r="T33">
+        <v>98233</v>
+      </c>
+      <c r="U33">
+        <v>35712</v>
+      </c>
+      <c r="V33" s="10">
+        <v>41043</v>
+      </c>
+      <c r="W33" s="10">
+        <v>30811</v>
+      </c>
+      <c r="X33">
+        <v>56155</v>
+      </c>
+      <c r="Y33">
+        <v>248841</v>
+      </c>
+      <c r="Z33">
+        <v>1435813</v>
+      </c>
+      <c r="AA33">
+        <v>1718000</v>
+      </c>
+      <c r="AD33">
+        <f>ABS(F33-R33)</f>
+        <v>36830</v>
+      </c>
+      <c r="AE33">
+        <f>ABS(G33-S33)</f>
+        <v>1210</v>
+      </c>
+      <c r="AF33">
+        <f>ABS(H33-T33)</f>
+        <v>4818</v>
+      </c>
+      <c r="AG33">
+        <f>ABS(I33-U33)</f>
+        <v>14426</v>
+      </c>
+      <c r="AH33">
+        <f>ABS(J33-V33)</f>
+        <v>7082</v>
+      </c>
+      <c r="AI33">
+        <f>ABS(K33-W33)</f>
+        <v>7693</v>
+      </c>
+      <c r="AJ33">
+        <f>ABS(L33-X33)</f>
+        <v>8113</v>
+      </c>
+      <c r="AK33">
+        <f>ABS(M33-Y33)</f>
+        <v>62309</v>
+      </c>
+      <c r="AL33">
+        <f>ABS(N33-Z33)</f>
+        <v>55805</v>
+      </c>
+      <c r="AM33">
+        <f>ABS(O33-AA33)</f>
+        <v>83920</v>
+      </c>
+    </row>
+    <row r="34" spans="5:39">
+      <c r="F34">
+        <v>1628025</v>
+      </c>
+      <c r="G34">
+        <v>855986</v>
+      </c>
+      <c r="H34">
+        <v>166987</v>
+      </c>
+      <c r="I34">
+        <v>54477</v>
+      </c>
+      <c r="J34" s="10">
+        <v>36767</v>
+      </c>
+      <c r="K34" s="10">
+        <v>43114</v>
+      </c>
+      <c r="L34">
+        <v>41692</v>
+      </c>
+      <c r="M34">
+        <v>180643</v>
+      </c>
+      <c r="N34">
+        <v>1501815</v>
+      </c>
+      <c r="O34">
+        <v>1619712</v>
+      </c>
+      <c r="R34">
+        <v>1516905</v>
+      </c>
+      <c r="S34">
+        <v>758369</v>
+      </c>
+      <c r="T34">
+        <v>115093</v>
+      </c>
+      <c r="U34">
+        <v>35068</v>
+      </c>
+      <c r="V34" s="10">
+        <v>31905</v>
+      </c>
+      <c r="W34" s="10">
+        <v>28248</v>
+      </c>
+      <c r="X34">
+        <v>29056</v>
+      </c>
+      <c r="Y34">
+        <v>184322</v>
+      </c>
+      <c r="Z34">
+        <v>1476703</v>
+      </c>
+      <c r="AA34">
+        <v>1636907</v>
+      </c>
+      <c r="AD34">
+        <f>ABS(F34-R34)</f>
+        <v>111120</v>
+      </c>
+      <c r="AE34">
+        <f>ABS(G34-S34)</f>
+        <v>97617</v>
+      </c>
+      <c r="AF34">
+        <f>ABS(H34-T34)</f>
+        <v>51894</v>
+      </c>
+      <c r="AG34">
+        <f>ABS(I34-U34)</f>
+        <v>19409</v>
+      </c>
+      <c r="AH34">
+        <f>ABS(J34-V34)</f>
+        <v>4862</v>
+      </c>
+      <c r="AI34">
+        <f>ABS(K34-W34)</f>
+        <v>14866</v>
+      </c>
+      <c r="AJ34">
+        <f>ABS(L34-X34)</f>
+        <v>12636</v>
+      </c>
+      <c r="AK34">
+        <f>ABS(M34-Y34)</f>
+        <v>3679</v>
+      </c>
+      <c r="AL34">
+        <f>ABS(N34-Z34)</f>
+        <v>25112</v>
+      </c>
+      <c r="AM34">
+        <f>ABS(O34-AA34)</f>
+        <v>17195</v>
+      </c>
+    </row>
+    <row r="35" spans="5:39">
+      <c r="F35">
+        <v>1770120</v>
+      </c>
+      <c r="G35">
+        <v>856498</v>
+      </c>
+      <c r="H35">
+        <v>236630</v>
+      </c>
+      <c r="I35">
+        <v>147159</v>
+      </c>
+      <c r="J35">
+        <v>105038</v>
+      </c>
+      <c r="K35">
+        <v>44824</v>
+      </c>
+      <c r="L35">
+        <v>42365</v>
+      </c>
+      <c r="M35">
+        <v>227599</v>
+      </c>
+      <c r="N35">
+        <v>1583309</v>
+      </c>
+      <c r="O35">
+        <v>1638560</v>
+      </c>
+      <c r="R35">
+        <v>1585964</v>
+      </c>
+      <c r="S35">
+        <v>701798</v>
+      </c>
+      <c r="T35">
+        <v>77090</v>
+      </c>
+      <c r="U35">
+        <v>22451</v>
+      </c>
+      <c r="V35">
+        <v>28109</v>
+      </c>
+      <c r="W35">
+        <v>40320</v>
+      </c>
+      <c r="X35">
+        <v>47442</v>
+      </c>
+      <c r="Y35">
+        <v>165802</v>
+      </c>
+      <c r="Z35">
+        <v>1519247</v>
+      </c>
+      <c r="AA35">
+        <v>1603153</v>
+      </c>
+      <c r="AD35">
+        <f>ABS(F35-R35)</f>
+        <v>184156</v>
+      </c>
+      <c r="AE35">
+        <f>ABS(G35-S35)</f>
+        <v>154700</v>
+      </c>
+      <c r="AF35">
+        <f>ABS(H35-T35)</f>
+        <v>159540</v>
+      </c>
+      <c r="AG35">
+        <f>ABS(I35-U35)</f>
+        <v>124708</v>
+      </c>
+      <c r="AH35">
+        <f>ABS(J35-V35)</f>
+        <v>76929</v>
+      </c>
+      <c r="AI35">
+        <f>ABS(K35-W35)</f>
+        <v>4504</v>
+      </c>
+      <c r="AJ35">
+        <f>ABS(L35-X35)</f>
+        <v>5077</v>
+      </c>
+      <c r="AK35">
+        <f>ABS(M35-Y35)</f>
+        <v>61797</v>
+      </c>
+      <c r="AL35">
+        <f>ABS(N35-Z35)</f>
+        <v>64062</v>
+      </c>
+      <c r="AM35">
+        <f>ABS(O35-AA35)</f>
+        <v>35407</v>
+      </c>
+    </row>
+    <row r="36" spans="5:39">
+      <c r="F36">
+        <v>2062591</v>
+      </c>
+      <c r="G36">
+        <v>1012875</v>
+      </c>
+      <c r="H36">
+        <v>379846</v>
+      </c>
+      <c r="I36">
+        <v>377826</v>
+      </c>
+      <c r="J36">
+        <v>408408</v>
+      </c>
+      <c r="K36">
+        <v>293586</v>
+      </c>
+      <c r="L36">
+        <v>220739</v>
+      </c>
+      <c r="M36">
+        <v>563882</v>
+      </c>
+      <c r="N36">
+        <v>1983144</v>
+      </c>
+      <c r="O36">
+        <v>1824937</v>
+      </c>
+      <c r="R36">
+        <v>1841670</v>
+      </c>
+      <c r="S36">
+        <v>989844</v>
+      </c>
+      <c r="T36">
+        <v>195373</v>
+      </c>
+      <c r="U36">
+        <v>98194</v>
+      </c>
+      <c r="V36">
+        <v>128119</v>
+      </c>
+      <c r="W36">
+        <v>172942</v>
+      </c>
+      <c r="X36">
+        <v>203614</v>
+      </c>
+      <c r="Y36">
+        <v>452067</v>
+      </c>
+      <c r="Z36">
+        <v>1902363</v>
+      </c>
+      <c r="AA36">
+        <v>1771723</v>
+      </c>
+      <c r="AD36">
+        <f>ABS(F36-R36)</f>
+        <v>220921</v>
+      </c>
+      <c r="AE36">
+        <f>ABS(G36-S36)</f>
+        <v>23031</v>
+      </c>
+      <c r="AF36">
+        <f>ABS(H36-T36)</f>
+        <v>184473</v>
+      </c>
+      <c r="AG36">
+        <f>ABS(I36-U36)</f>
+        <v>279632</v>
+      </c>
+      <c r="AH36">
+        <f>ABS(J36-V36)</f>
+        <v>280289</v>
+      </c>
+      <c r="AI36">
+        <f>ABS(K36-W36)</f>
+        <v>120644</v>
+      </c>
+      <c r="AJ36">
+        <f>ABS(L36-X36)</f>
+        <v>17125</v>
+      </c>
+      <c r="AK36">
+        <f>ABS(M36-Y36)</f>
+        <v>111815</v>
+      </c>
+      <c r="AL36">
+        <f>ABS(N36-Z36)</f>
+        <v>80781</v>
+      </c>
+      <c r="AM36">
+        <f>ABS(O36-AA36)</f>
+        <v>53214</v>
+      </c>
+    </row>
+    <row r="37" spans="5:39">
+      <c r="F37">
+        <v>3009631</v>
+      </c>
+      <c r="G37">
+        <v>2104486</v>
+      </c>
+      <c r="H37">
+        <v>1356624</v>
+      </c>
+      <c r="I37">
+        <v>1388108</v>
+      </c>
+      <c r="J37">
+        <v>1553115</v>
+      </c>
+      <c r="K37">
+        <v>1579697</v>
+      </c>
+      <c r="L37">
+        <v>1554310</v>
+      </c>
+      <c r="M37">
+        <v>1865357</v>
+      </c>
+      <c r="N37">
+        <v>2899958</v>
+      </c>
+      <c r="O37">
+        <v>2563366</v>
+      </c>
+      <c r="R37">
+        <v>2678544</v>
+      </c>
+      <c r="S37">
+        <v>2150766</v>
+      </c>
+      <c r="T37">
+        <v>1315961</v>
+      </c>
+      <c r="U37">
+        <v>1101709</v>
+      </c>
+      <c r="V37">
+        <v>1161913</v>
+      </c>
+      <c r="W37">
+        <v>1247624</v>
+      </c>
+      <c r="X37">
+        <v>1330510</v>
+      </c>
+      <c r="Y37">
+        <v>1774323</v>
+      </c>
+      <c r="Z37">
+        <v>2840294</v>
+      </c>
+      <c r="AA37">
+        <v>2501530</v>
+      </c>
+      <c r="AD37">
+        <f>ABS(F37-R37)</f>
+        <v>331087</v>
+      </c>
+      <c r="AE37">
+        <f>ABS(G37-S37)</f>
+        <v>46280</v>
+      </c>
+      <c r="AF37">
+        <f>ABS(H37-T37)</f>
+        <v>40663</v>
+      </c>
+      <c r="AG37">
+        <f>ABS(I37-U37)</f>
+        <v>286399</v>
+      </c>
+      <c r="AH37">
+        <f>ABS(J37-V37)</f>
+        <v>391202</v>
+      </c>
+      <c r="AI37">
+        <f>ABS(K37-W37)</f>
+        <v>332073</v>
+      </c>
+      <c r="AJ37">
+        <f>ABS(L37-X37)</f>
+        <v>223800</v>
+      </c>
+      <c r="AK37">
+        <f>ABS(M37-Y37)</f>
+        <v>91034</v>
+      </c>
+      <c r="AL37">
+        <f>ABS(N37-Z37)</f>
+        <v>59664</v>
+      </c>
+      <c r="AM37">
+        <f>ABS(O37-AA37)</f>
+        <v>61836</v>
+      </c>
+    </row>
+    <row r="38" spans="5:39">
+      <c r="F38">
+        <v>1758749</v>
+      </c>
+      <c r="G38">
+        <v>2402998</v>
+      </c>
+      <c r="H38">
+        <v>1801292</v>
+      </c>
+      <c r="I38">
+        <v>1729650</v>
+      </c>
+      <c r="J38">
+        <v>1648740</v>
+      </c>
+      <c r="K38">
+        <v>1569209</v>
+      </c>
+      <c r="L38">
+        <v>1538643</v>
+      </c>
+      <c r="M38">
+        <v>1697730</v>
+      </c>
+      <c r="N38">
+        <v>2410504</v>
+      </c>
+      <c r="O38">
+        <v>1066224</v>
+      </c>
+      <c r="R38">
+        <v>1621656</v>
+      </c>
+      <c r="S38">
+        <v>2115915</v>
+      </c>
+      <c r="T38">
+        <v>1615987</v>
+      </c>
+      <c r="U38">
+        <v>1574148</v>
+      </c>
+      <c r="V38">
+        <v>1552138</v>
+      </c>
+      <c r="W38">
+        <v>1505682</v>
+      </c>
+      <c r="X38">
+        <v>1482402</v>
+      </c>
+      <c r="Y38">
+        <v>1651676</v>
+      </c>
+      <c r="Z38">
+        <v>2365818</v>
+      </c>
+      <c r="AA38">
+        <v>1059240</v>
+      </c>
+      <c r="AD38">
+        <f>ABS(F38-R38)</f>
+        <v>137093</v>
+      </c>
+      <c r="AE38">
+        <f>ABS(G38-S38)</f>
+        <v>287083</v>
+      </c>
+      <c r="AF38">
+        <f>ABS(H38-T38)</f>
+        <v>185305</v>
+      </c>
+      <c r="AG38">
+        <f>ABS(I38-U38)</f>
+        <v>155502</v>
+      </c>
+      <c r="AH38">
+        <f>ABS(J38-V38)</f>
+        <v>96602</v>
+      </c>
+      <c r="AI38">
+        <f>ABS(K38-W38)</f>
+        <v>63527</v>
+      </c>
+      <c r="AJ38">
+        <f>ABS(L38-X38)</f>
+        <v>56241</v>
+      </c>
+      <c r="AK38">
+        <f>ABS(M38-Y38)</f>
+        <v>46054</v>
+      </c>
+      <c r="AL38">
+        <f>ABS(N38-Z38)</f>
+        <v>44686</v>
+      </c>
+      <c r="AM38">
+        <f>ABS(O38-AA38)</f>
+        <v>6984</v>
+      </c>
+    </row>
+    <row r="39" spans="5:39">
+      <c r="E39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>100</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>3</v>
+      </c>
+      <c r="R39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="5:39">
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" t="s">
+        <v>37</v>
+      </c>
+      <c r="J40" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>8</v>
+      </c>
+      <c r="R40" t="s">
+        <v>9</v>
+      </c>
+      <c r="S40" t="s">
+        <v>10</v>
+      </c>
+      <c r="T40" t="s">
+        <v>11</v>
+      </c>
+      <c r="U40" t="s">
+        <v>38</v>
+      </c>
+      <c r="V40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="5:39">
+      <c r="F44">
+        <f>ABS(F29-F10)</f>
+        <v>250316</v>
+      </c>
+      <c r="G44">
+        <f t="shared" ref="G44:O44" si="0">ABS(G29-G10)</f>
+        <v>423263</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>195409</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>105314</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="0"/>
+        <v>16918</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="0"/>
+        <v>100064</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="0"/>
+        <v>118147</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="0"/>
+        <v>87489</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="0"/>
+        <v>100220</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="0"/>
+        <v>7136</v>
+      </c>
+      <c r="R44">
+        <f t="shared" ref="R44:AA44" si="1">ABS(R29-R10)</f>
+        <v>45372</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="1"/>
+        <v>114341</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="1"/>
+        <v>43504</v>
+      </c>
+      <c r="U44">
+        <f t="shared" si="1"/>
+        <v>33168</v>
+      </c>
+      <c r="V44">
+        <f t="shared" si="1"/>
+        <v>181100</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="1"/>
+        <v>318314</v>
+      </c>
+      <c r="X44">
+        <f t="shared" si="1"/>
+        <v>370436</v>
+      </c>
+      <c r="Y44">
+        <f t="shared" si="1"/>
+        <v>285180</v>
+      </c>
+      <c r="Z44">
+        <f t="shared" si="1"/>
+        <v>323277</v>
+      </c>
+      <c r="AA44">
+        <f t="shared" si="1"/>
+        <v>19473</v>
+      </c>
+    </row>
+    <row r="45" spans="5:39">
+      <c r="F45">
+        <f t="shared" ref="F45:O45" si="2">ABS(F30-F11)</f>
+        <v>674781</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="2"/>
+        <v>140032</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="2"/>
+        <v>155068</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="2"/>
+        <v>102315</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="2"/>
+        <v>134961</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="2"/>
+        <v>167410</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="2"/>
+        <v>193518</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="2"/>
+        <v>307675</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="2"/>
+        <v>305552</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="2"/>
+        <v>213073</v>
+      </c>
+      <c r="R45">
+        <f t="shared" ref="R45:AA45" si="3">ABS(R30-R11)</f>
+        <v>153682</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="3"/>
+        <v>311927</v>
+      </c>
+      <c r="T45">
+        <f t="shared" si="3"/>
+        <v>319167</v>
+      </c>
+      <c r="U45">
+        <f t="shared" si="3"/>
+        <v>242315</v>
+      </c>
+      <c r="V45">
+        <f t="shared" si="3"/>
+        <v>261303</v>
+      </c>
+      <c r="W45">
+        <f t="shared" si="3"/>
+        <v>263984</v>
+      </c>
+      <c r="X45">
+        <f t="shared" si="3"/>
+        <v>98134</v>
+      </c>
+      <c r="Y45">
+        <f t="shared" si="3"/>
+        <v>265288</v>
+      </c>
+      <c r="Z45">
+        <f t="shared" si="3"/>
+        <v>404099</v>
+      </c>
+      <c r="AA45">
+        <f t="shared" si="3"/>
+        <v>492603</v>
+      </c>
+    </row>
+    <row r="46" spans="5:39">
+      <c r="F46">
+        <f t="shared" ref="F46:O46" si="4">ABS(F31-F12)</f>
+        <v>569241</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="4"/>
+        <v>98443</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="4"/>
+        <v>127219</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="4"/>
+        <v>111688</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="4"/>
+        <v>66560</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="4"/>
+        <v>31127</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="4"/>
+        <v>44136</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="4"/>
+        <v>143724</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="4"/>
+        <v>394708</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="4"/>
+        <v>130127</v>
+      </c>
+      <c r="R46">
+        <f t="shared" ref="R46:AA46" si="5">ABS(R31-R12)</f>
+        <v>137821</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="5"/>
+        <v>361755</v>
+      </c>
+      <c r="T46">
+        <f t="shared" si="5"/>
+        <v>111432</v>
+      </c>
+      <c r="U46">
+        <f t="shared" si="5"/>
+        <v>12343</v>
+      </c>
+      <c r="V46">
+        <f t="shared" si="5"/>
+        <v>81449</v>
+      </c>
+      <c r="W46">
+        <f t="shared" si="5"/>
+        <v>220587</v>
+      </c>
+      <c r="X46">
+        <f t="shared" si="5"/>
+        <v>166185</v>
+      </c>
+      <c r="Y46">
+        <f t="shared" si="5"/>
+        <v>33787</v>
+      </c>
+      <c r="Z46">
+        <f t="shared" si="5"/>
+        <v>554061</v>
+      </c>
+      <c r="AA46">
+        <f t="shared" si="5"/>
+        <v>290728</v>
+      </c>
+    </row>
+    <row r="47" spans="5:39">
+      <c r="F47">
+        <f t="shared" ref="F47:O47" si="6">ABS(F32-F13)</f>
+        <v>526772</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="6"/>
+        <v>205730</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="6"/>
+        <v>210123</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="6"/>
+        <v>87261</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="6"/>
+        <v>8866</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="6"/>
+        <v>4036</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="6"/>
+        <v>14139</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="6"/>
+        <v>45732</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="6"/>
+        <v>158199</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="6"/>
+        <v>53413</v>
+      </c>
+      <c r="R47">
+        <f t="shared" ref="R47:AA47" si="7">ABS(R32-R13)</f>
+        <v>175107</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="7"/>
+        <v>231634</v>
+      </c>
+      <c r="T47">
+        <f t="shared" si="7"/>
+        <v>34204</v>
+      </c>
+      <c r="U47">
+        <f t="shared" si="7"/>
+        <v>3897</v>
+      </c>
+      <c r="V47">
+        <f t="shared" si="7"/>
+        <v>703</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="7"/>
+        <v>67489</v>
+      </c>
+      <c r="X47">
+        <f t="shared" si="7"/>
+        <v>97357</v>
+      </c>
+      <c r="Y47">
+        <f t="shared" si="7"/>
+        <v>73033</v>
+      </c>
+      <c r="Z47">
+        <f t="shared" si="7"/>
+        <v>333608</v>
+      </c>
+      <c r="AA47">
+        <f t="shared" si="7"/>
+        <v>166950</v>
+      </c>
+    </row>
+    <row r="48" spans="5:39">
+      <c r="F48">
+        <f t="shared" ref="F48:O48" si="8">ABS(F33-F14)</f>
+        <v>293606</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="8"/>
+        <v>261737</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="8"/>
+        <v>175603</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="8"/>
+        <v>52192</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="8"/>
+        <v>180</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="8"/>
+        <v>5049</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="8"/>
+        <v>12588</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="8"/>
+        <v>29671</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="8"/>
+        <v>64159</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="8"/>
+        <v>71182</v>
+      </c>
+      <c r="R48">
+        <f t="shared" ref="R48:AA48" si="9">ABS(R33-R14)</f>
+        <v>150321</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="9"/>
+        <v>145185</v>
+      </c>
+      <c r="T48">
+        <f t="shared" si="9"/>
+        <v>36912</v>
+      </c>
+      <c r="U48">
+        <f t="shared" si="9"/>
+        <v>13208</v>
+      </c>
+      <c r="V48">
+        <f t="shared" si="9"/>
+        <v>1845</v>
+      </c>
+      <c r="W48">
+        <f t="shared" si="9"/>
+        <v>9945</v>
+      </c>
+      <c r="X48">
+        <f t="shared" si="9"/>
+        <v>6386</v>
+      </c>
+      <c r="Y48">
+        <f t="shared" si="9"/>
+        <v>103683</v>
+      </c>
+      <c r="Z48">
+        <f t="shared" si="9"/>
+        <v>234176</v>
+      </c>
+      <c r="AA48">
+        <f t="shared" si="9"/>
+        <v>56384</v>
+      </c>
+    </row>
+    <row r="49" spans="6:27">
+      <c r="F49">
+        <f t="shared" ref="F49:O49" si="10">ABS(F34-F15)</f>
+        <v>6132</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="10"/>
+        <v>172048</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="10"/>
+        <v>17634</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="10"/>
+        <v>22574</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="10"/>
+        <v>8129</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="10"/>
+        <v>10185</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="10"/>
+        <v>19729</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="10"/>
+        <v>69894</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="10"/>
+        <v>273410</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="10"/>
+        <v>140512</v>
+      </c>
+      <c r="R49">
+        <f t="shared" ref="R49:AA49" si="11">ABS(R34-R15)</f>
+        <v>41890</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="11"/>
+        <v>8844</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="11"/>
+        <v>15180</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="11"/>
+        <v>3489</v>
+      </c>
+      <c r="V49">
+        <f t="shared" si="11"/>
+        <v>3201</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="11"/>
+        <v>14157</v>
+      </c>
+      <c r="X49">
+        <f t="shared" si="11"/>
+        <v>107034</v>
+      </c>
+      <c r="Y49">
+        <f t="shared" si="11"/>
+        <v>236098</v>
+      </c>
+      <c r="Z49">
+        <f t="shared" si="11"/>
+        <v>86026</v>
+      </c>
+      <c r="AA49">
+        <f t="shared" si="11"/>
+        <v>307299</v>
+      </c>
+    </row>
+    <row r="50" spans="6:27">
+      <c r="F50">
+        <f t="shared" ref="F50:O50" si="12">ABS(F35-F16)</f>
+        <v>249100</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="12"/>
+        <v>138734</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="12"/>
+        <v>152774</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="12"/>
+        <v>113232</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="12"/>
+        <v>59986</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="12"/>
+        <v>2064</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="12"/>
+        <v>18421</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="12"/>
+        <v>131770</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="12"/>
+        <v>378334</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="12"/>
+        <v>140889</v>
+      </c>
+      <c r="R50">
+        <f t="shared" ref="R50:AA50" si="13">ABS(R35-R16)</f>
+        <v>96312</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="13"/>
+        <v>131338</v>
+      </c>
+      <c r="T50">
+        <f t="shared" si="13"/>
+        <v>47045</v>
+      </c>
+      <c r="U50">
+        <f t="shared" si="13"/>
+        <v>14052</v>
+      </c>
+      <c r="V50">
+        <f t="shared" si="13"/>
+        <v>869</v>
+      </c>
+      <c r="W50">
+        <f t="shared" si="13"/>
+        <v>35896</v>
+      </c>
+      <c r="X50">
+        <f t="shared" si="13"/>
+        <v>113321</v>
+      </c>
+      <c r="Y50">
+        <f t="shared" si="13"/>
+        <v>187280</v>
+      </c>
+      <c r="Z50">
+        <f t="shared" si="13"/>
+        <v>141264</v>
+      </c>
+      <c r="AA50">
+        <f t="shared" si="13"/>
+        <v>488232</v>
+      </c>
+    </row>
+    <row r="51" spans="6:27">
+      <c r="F51">
+        <f t="shared" ref="F51:O51" si="14">ABS(F36-F17)</f>
+        <v>337041</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="14"/>
+        <v>352908</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="14"/>
+        <v>11512</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="14"/>
+        <v>197077</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="14"/>
+        <v>228074</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="14"/>
+        <v>113632</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="14"/>
+        <v>94061</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="14"/>
+        <v>283738</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="14"/>
+        <v>476008</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="14"/>
+        <v>107808</v>
+      </c>
+      <c r="R51">
+        <f t="shared" ref="R51:AA51" si="15">ABS(R36-R17)</f>
+        <v>154908</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="15"/>
+        <v>312308</v>
+      </c>
+      <c r="T51">
+        <f t="shared" si="15"/>
+        <v>111145</v>
+      </c>
+      <c r="U51">
+        <f t="shared" si="15"/>
+        <v>56544</v>
+      </c>
+      <c r="V51">
+        <f t="shared" si="15"/>
+        <v>70831</v>
+      </c>
+      <c r="W51">
+        <f t="shared" si="15"/>
+        <v>91010</v>
+      </c>
+      <c r="X51">
+        <f t="shared" si="15"/>
+        <v>100342</v>
+      </c>
+      <c r="Y51">
+        <f t="shared" si="15"/>
+        <v>29365</v>
+      </c>
+      <c r="Z51">
+        <f t="shared" si="15"/>
+        <v>480480</v>
+      </c>
+      <c r="AA51">
+        <f t="shared" si="15"/>
+        <v>486824</v>
+      </c>
+    </row>
+    <row r="52" spans="6:27">
+      <c r="F52">
+        <f t="shared" ref="F52:O52" si="16">ABS(F37-F18)</f>
+        <v>466639</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="16"/>
+        <v>397491</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="16"/>
+        <v>381071</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="16"/>
+        <v>10507</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="16"/>
+        <v>227052</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="16"/>
+        <v>372447</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="16"/>
+        <v>425983</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="16"/>
+        <v>462204</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="16"/>
+        <v>368431</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="16"/>
+        <v>125424</v>
+      </c>
+      <c r="R52">
+        <f t="shared" ref="R52:AA52" si="17">ABS(R37-R18)</f>
+        <v>193930</v>
+      </c>
+      <c r="S52">
+        <f t="shared" si="17"/>
+        <v>266540</v>
+      </c>
+      <c r="T52">
+        <f t="shared" si="17"/>
+        <v>319808</v>
+      </c>
+      <c r="U52">
+        <f t="shared" si="17"/>
+        <v>231654</v>
+      </c>
+      <c r="V52">
+        <f t="shared" si="17"/>
+        <v>178410</v>
+      </c>
+      <c r="W52">
+        <f t="shared" si="17"/>
+        <v>55955</v>
+      </c>
+      <c r="X52">
+        <f t="shared" si="17"/>
+        <v>95132</v>
+      </c>
+      <c r="Y52">
+        <f t="shared" si="17"/>
+        <v>446642</v>
+      </c>
+      <c r="Z52">
+        <f t="shared" si="17"/>
+        <v>454755</v>
+      </c>
+      <c r="AA52">
+        <f t="shared" si="17"/>
+        <v>574404</v>
+      </c>
+    </row>
+    <row r="53" spans="6:27">
+      <c r="F53">
+        <f t="shared" ref="F53:O53" si="18">ABS(F38-F19)</f>
+        <v>166321</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="18"/>
+        <v>361788</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="18"/>
+        <v>227606</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="18"/>
+        <v>218815</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="18"/>
+        <v>145754</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="18"/>
+        <v>62363</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="18"/>
+        <v>3499</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="18"/>
+        <v>8440</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="18"/>
+        <v>44633</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="18"/>
+        <v>21834</v>
+      </c>
+      <c r="R53">
+        <f t="shared" ref="R53:AA53" si="19">ABS(R38-R19)</f>
+        <v>49785</v>
+      </c>
+      <c r="S53">
+        <f t="shared" si="19"/>
+        <v>119037</v>
+      </c>
+      <c r="T53">
+        <f t="shared" si="19"/>
+        <v>72877</v>
+      </c>
+      <c r="U53">
+        <f t="shared" si="19"/>
+        <v>70566</v>
+      </c>
+      <c r="V53">
+        <f t="shared" si="19"/>
+        <v>14458</v>
+      </c>
+      <c r="W53">
+        <f t="shared" si="19"/>
+        <v>78395</v>
+      </c>
+      <c r="X53">
+        <f t="shared" si="19"/>
+        <v>162968</v>
+      </c>
+      <c r="Y53">
+        <f t="shared" si="19"/>
+        <v>158918</v>
+      </c>
+      <c r="Z53">
+        <f t="shared" si="19"/>
+        <v>271357</v>
+      </c>
+      <c r="AA53">
+        <f t="shared" si="19"/>
+        <v>6944</v>
+      </c>
+    </row>
+    <row r="54" spans="6:27">
+      <c r="F54">
+        <f t="shared" ref="F54:O54" si="20">ABS(F39-F20)</f>
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <f t="shared" ref="R54:AA54" si="21">ABS(R39-R20)</f>
+        <v>0</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T54">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="U54">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="V54">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="W54">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="X54">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="Y54">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="Z54">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AA54">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F10:O19 R10:AA19 R29:AA38 F29:O38">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD10">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD10:AM19">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD29:AM38">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44:O54">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R44:AA54">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Wavelets compression and decompression test
</commit_message>
<xml_diff>
--- a/Reports/test data 2 (version2).xlsx
+++ b/Reports/test data 2 (version2).xlsx
@@ -15954,10 +15954,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C1:AJ83"/>
+  <dimension ref="C1:AJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="W89" sqref="W89"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="O93" sqref="O93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21341,7 +21341,386 @@
         <v>45100</v>
       </c>
     </row>
+    <row r="92" spans="4:25">
+      <c r="D92">
+        <f t="shared" ref="D92:M100" si="60">ABS(D25-D43)</f>
+        <v>62671</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="60"/>
+        <v>197353</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="60"/>
+        <v>180695</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="60"/>
+        <v>101349</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="60"/>
+        <v>1000</v>
+      </c>
+      <c r="I92">
+        <f t="shared" si="60"/>
+        <v>69816</v>
+      </c>
+      <c r="J92">
+        <f t="shared" si="60"/>
+        <v>118730</v>
+      </c>
+      <c r="K92">
+        <f t="shared" si="60"/>
+        <v>153992</v>
+      </c>
+      <c r="L92">
+        <f t="shared" si="60"/>
+        <v>195089</v>
+      </c>
+      <c r="M92">
+        <f t="shared" si="60"/>
+        <v>162703</v>
+      </c>
+    </row>
+    <row r="93" spans="4:25">
+      <c r="D93">
+        <f t="shared" ref="D93:M100" si="61">ABS(D26-D44)</f>
+        <v>211778</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="61"/>
+        <v>413032</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="61"/>
+        <v>373344</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="61"/>
+        <v>267127</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="61"/>
+        <v>151657</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="61"/>
+        <v>74585</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="61"/>
+        <v>13952</v>
+      </c>
+      <c r="K93">
+        <f t="shared" si="61"/>
+        <v>29185</v>
+      </c>
+      <c r="L93">
+        <f t="shared" si="61"/>
+        <v>45879</v>
+      </c>
+      <c r="M93">
+        <f t="shared" si="61"/>
+        <v>7302</v>
+      </c>
+    </row>
+    <row r="94" spans="4:25">
+      <c r="D94">
+        <f t="shared" ref="D94:M100" si="62">ABS(D27-D45)</f>
+        <v>187948</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="62"/>
+        <v>365551</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="62"/>
+        <v>325129</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="62"/>
+        <v>236878</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="62"/>
+        <v>116093</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="62"/>
+        <v>33501</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="62"/>
+        <v>31162</v>
+      </c>
+      <c r="K94">
+        <f t="shared" si="62"/>
+        <v>86680</v>
+      </c>
+      <c r="L94">
+        <f t="shared" si="62"/>
+        <v>129904</v>
+      </c>
+      <c r="M94">
+        <f t="shared" si="62"/>
+        <v>41522</v>
+      </c>
+    </row>
+    <row r="95" spans="4:25">
+      <c r="D95">
+        <f t="shared" ref="D95:M100" si="63">ABS(D28-D46)</f>
+        <v>178504</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="63"/>
+        <v>337504</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="63"/>
+        <v>293689</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="63"/>
+        <v>228086</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="63"/>
+        <v>130379</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="63"/>
+        <v>35619</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="63"/>
+        <v>44447</v>
+      </c>
+      <c r="K95">
+        <f t="shared" si="63"/>
+        <v>117349</v>
+      </c>
+      <c r="L95">
+        <f t="shared" si="63"/>
+        <v>165111</v>
+      </c>
+      <c r="M95">
+        <f t="shared" si="63"/>
+        <v>51787</v>
+      </c>
+    </row>
+    <row r="96" spans="4:25">
+      <c r="D96">
+        <f t="shared" ref="D96:M100" si="64">ABS(D29-D47)</f>
+        <v>168597</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="64"/>
+        <v>291474</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="64"/>
+        <v>235425</v>
+      </c>
+      <c r="G96">
+        <f t="shared" si="64"/>
+        <v>171784</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="64"/>
+        <v>86753</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="64"/>
+        <v>1707</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="64"/>
+        <v>61246</v>
+      </c>
+      <c r="K96">
+        <f t="shared" si="64"/>
+        <v>120141</v>
+      </c>
+      <c r="L96">
+        <f t="shared" si="64"/>
+        <v>182762</v>
+      </c>
+      <c r="M96">
+        <f t="shared" si="64"/>
+        <v>60430</v>
+      </c>
+    </row>
+    <row r="97" spans="4:13">
+      <c r="D97">
+        <f t="shared" ref="D97:M100" si="65">ABS(D30-D48)</f>
+        <v>136289</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="65"/>
+        <v>208839</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="65"/>
+        <v>146741</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="65"/>
+        <v>83969</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="65"/>
+        <v>16463</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="65"/>
+        <v>35187</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="65"/>
+        <v>60383</v>
+      </c>
+      <c r="K97">
+        <f t="shared" si="65"/>
+        <v>118196</v>
+      </c>
+      <c r="L97">
+        <f t="shared" si="65"/>
+        <v>173048</v>
+      </c>
+      <c r="M97">
+        <f t="shared" si="65"/>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="98" spans="4:13">
+      <c r="D98">
+        <f t="shared" ref="D98:M100" si="66">ABS(D31-D49)</f>
+        <v>39778</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="66"/>
+        <v>53521</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="66"/>
+        <v>10951</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="66"/>
+        <v>86155</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="66"/>
+        <v>119170</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="66"/>
+        <v>139258</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="66"/>
+        <v>171250</v>
+      </c>
+      <c r="K98">
+        <f t="shared" si="66"/>
+        <v>214552</v>
+      </c>
+      <c r="L98">
+        <f t="shared" si="66"/>
+        <v>261255</v>
+      </c>
+      <c r="M98">
+        <f t="shared" si="66"/>
+        <v>96429</v>
+      </c>
+    </row>
+    <row r="99" spans="4:13">
+      <c r="D99">
+        <f t="shared" ref="D99:M100" si="67">ABS(D32-D50)</f>
+        <v>60611</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="67"/>
+        <v>69578</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="67"/>
+        <v>107185</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="67"/>
+        <v>134598</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="67"/>
+        <v>145384</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="67"/>
+        <v>150202</v>
+      </c>
+      <c r="J99">
+        <f t="shared" si="67"/>
+        <v>158885</v>
+      </c>
+      <c r="K99">
+        <f t="shared" si="67"/>
+        <v>173993</v>
+      </c>
+      <c r="L99">
+        <f t="shared" si="67"/>
+        <v>159944</v>
+      </c>
+      <c r="M99">
+        <f t="shared" si="67"/>
+        <v>71672</v>
+      </c>
+    </row>
+    <row r="100" spans="4:13">
+      <c r="D100">
+        <f t="shared" ref="D100:M101" si="68">ABS(D33-D51)</f>
+        <v>195314</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="68"/>
+        <v>125602</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="68"/>
+        <v>56319</v>
+      </c>
+      <c r="G100">
+        <f t="shared" si="68"/>
+        <v>41076</v>
+      </c>
+      <c r="H100">
+        <f t="shared" si="68"/>
+        <v>37672</v>
+      </c>
+      <c r="I100">
+        <f t="shared" si="68"/>
+        <v>38318</v>
+      </c>
+      <c r="J100">
+        <f t="shared" si="68"/>
+        <v>41228</v>
+      </c>
+      <c r="K100">
+        <f t="shared" si="68"/>
+        <v>48619</v>
+      </c>
+      <c r="L100">
+        <f t="shared" si="68"/>
+        <v>130039</v>
+      </c>
+      <c r="M100">
+        <f t="shared" si="68"/>
+        <v>205232</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>